<commit_message>
Created/compilaed  dictionary pt_br and en_us
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Texto</t>
   </si>
@@ -25,154 +25,151 @@
     <t>Porcentagem de erro ortográfico</t>
   </si>
   <si>
+    <t>10 razões pelas quais não deveria vacinar seu filho.txt</t>
+  </si>
+  <si>
+    <t>Aftas são a causa do câncer.txt</t>
+  </si>
+  <si>
+    <t>Ar condicionado e o benzeno.txt</t>
+  </si>
+  <si>
+    <t>Aspartame causa esclerose múltipla e lúpus.txt</t>
+  </si>
+  <si>
+    <t>Associação Americana e causas do câncer.txt</t>
+  </si>
+  <si>
+    <t>Banho frio e desmaios.txt</t>
+  </si>
+  <si>
+    <t>Beber água de estômago vazio faz bem à saúde e mais do que isso cura doenças inclusive o câncer.txt</t>
+  </si>
+  <si>
+    <t>Chá de erva doce e o tratamento do novo coronavírus.txt</t>
+  </si>
+  <si>
+    <t>Consumo de Skol e problemas renais ou câncer.txt</t>
+  </si>
+  <si>
+    <t>Consumo de fanta e coca e problemas renais ou câncer.txt</t>
+  </si>
+  <si>
+    <t>Cura do câncer.txt</t>
+  </si>
+  <si>
+    <t>Câncer é deficiência da vitamina B17.txt</t>
+  </si>
+  <si>
+    <t>Equinócio e altas temperaturas.txt</t>
+  </si>
+  <si>
+    <t>Gelo causa câncer.txt</t>
+  </si>
+  <si>
+    <t>História sobre o arroz Dana estar contaminado por um vírus.txt</t>
+  </si>
+  <si>
+    <t>Limão no copo mata.txt</t>
+  </si>
+  <si>
+    <t>Notificação emergencial do Ministério da Saúde sobre novo coronavírus.txt</t>
+  </si>
+  <si>
+    <t>Nova doença.txt</t>
+  </si>
+  <si>
+    <t>Ondas radioativas do microondas causam danos à saúde.txt</t>
+  </si>
+  <si>
+    <t>Situação fora de controle novo coronavírus.txt</t>
+  </si>
+  <si>
+    <t>Tossir evita infarto.txt</t>
+  </si>
+  <si>
+    <t>Tratamento de queimaduras com farinha de trigo.txt</t>
+  </si>
+  <si>
+    <t>Uso de celular na cozinha e acidentes.txt</t>
+  </si>
+  <si>
+    <t>Uísque e mel contra coronavírus.txt</t>
+  </si>
+  <si>
     <t>Água quente com abacaxi.txt</t>
   </si>
   <si>
-    <t>Beber água de estômago vazio faz bem à saúde e mais do que isso cura doenças inclusive o câncer.txt</t>
-  </si>
-  <si>
-    <t>Uso de celular na cozinha e acidentes.txt</t>
-  </si>
-  <si>
-    <t>Tratamento de queimaduras com farinha de trigo.txt</t>
-  </si>
-  <si>
-    <t>Equinócio e altas temperaturas.txt</t>
-  </si>
-  <si>
-    <t>Aspartame causa esclerose múltipla e lúpus.txt</t>
-  </si>
-  <si>
-    <t>Notificação emergencial do Ministério da Saúde sobre novo coronavírus.txt</t>
-  </si>
-  <si>
-    <t>Aftas são a causa do câncer.txt</t>
-  </si>
-  <si>
-    <t>Nova doença.txt</t>
-  </si>
-  <si>
-    <t>Tossir evita infarto.txt</t>
-  </si>
-  <si>
-    <t>Associação Americana e causas do câncer.txt</t>
-  </si>
-  <si>
-    <t>10 razões pelas quais não deveria vacinar seu filho.txt</t>
-  </si>
-  <si>
-    <t>Banho frio e desmaios.txt</t>
-  </si>
-  <si>
-    <t>Consumo de Skol e problemas renais ou câncer.txt</t>
-  </si>
-  <si>
-    <t>Cura do câncer.txt</t>
-  </si>
-  <si>
-    <t>Uísque e mel contra coronavírus.txt</t>
-  </si>
-  <si>
-    <t>Situação fora de controle novo coronavírus.txt</t>
-  </si>
-  <si>
-    <t>Câncer é deficiência da vitamina B17.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Consumo de fanta e coca e problemas renais ou câncer.txt</t>
-  </si>
-  <si>
-    <t>Gelo causa câncer.txt</t>
-  </si>
-  <si>
-    <t>Ar condicionado e o benzeno.txt</t>
-  </si>
-  <si>
-    <t>História sobre o arroz Dana estar contaminado por um vírus.txt</t>
-  </si>
-  <si>
-    <t>Limão no copo mata.txt</t>
-  </si>
-  <si>
-    <t>Ondas radioativas do microondas causam danos à saúde.txt</t>
-  </si>
-  <si>
-    <t>Chá de erva doce e o tratamento do novo coronavírus.txt</t>
-  </si>
-  <si>
-    <t>cistos, ”, extrato, enfatizou, anticâncer, polifenóis, .., “, …, huiren, alcalina</t>
-  </si>
-  <si>
-    <t>solidifica, urinário, gastrite, retarda, menstruais, obstipação, reparte-se, ..., divulgamos, 'mistura</t>
-  </si>
-  <si>
-    <t>3-4, lembre-se, afaste-se, ..., ademola</t>
-  </si>
-  <si>
-    <t>tirei-a, antioxidantes, extinguiu, fervente, compartilhá-lo, ..., reencaminhado</t>
-  </si>
-  <si>
-    <t>indicativos, outros…, 11h, freqüente, 16h</t>
-  </si>
-  <si>
-    <t>internadas, 9,5, mancy, repasse, adiposas, 'se, endossar, '', sistêmico, articulares, dietético, arckle, dietética, dr., fetais, agravando, equal, zerocal, atrapalhada, raffaele, riccio, 9975-4476, 30º, lobbies, carta-posição, spoonful, alimentícia, 3078-0995, apresentavam, comercializem, câimbras, malformações, entitulado, citados, colocá-la, suplanta, engaje, assolassem, fórmico, h.j, formigamento, assintomáticas, aspartame, ``, nutrasweet, fibromialgia</t>
-  </si>
-  <si>
-    <t>influenza, úmida, 50-80cc, propensas, c., 30-50cc, invadirá, coronavírus</t>
-  </si>
-  <si>
-    <t>candidíase, aplaudido, albicans, carcinosi, charcot, enlouquecida, menstruações, ___________________________________________________________, tumore, endossando, deleto, vari, adenocarcinoma, bronchiale, colecisti, enema, 20-30-40, removê-la, coróide, revolucionando, nahco3, inalações, embasamento, complementá-la, percebíamos, aftas, tanti, não-hodgkin, 90°, cancerologia, acentuado, professores-doutores-catedráticos-phds, pecezinho, 36a, mangueirinha, aproveitável, cânceres, oncologistas, usa-se, 70-100, ovo-de-colombo, ``, subsequentemente, mês.1, picaretagem, alternada, epatocarcinoma, urinaria, integradores, oriundos, aprofundando, cervice, persistirem, arteriografia, ..., acidificando, novembro/2008, .todos, linfomas, gravem, efetuar, praticadas, peritonial, charlatanismo, apregoam, prostata, 'delete, câncer/2008, peritoneale, metodologias, ingerível, difusível, caixa-postal, jfj, experimente-a, vezes.1, ministrando, posicionar-se, comprovam, 1/2, alla, lincados, conseqüência, causal, //www.curenaturalicancro.org/terapiasimoncinii…/bic.htm, intersticial, paradigmas, especificas, disseminação, simoncini, homeopatia, dias.3, engoli-la, --, helsinque, casi, convicta, conjuntiva, turmores, axilares, didática, administrá-lo, baseia-se, tullio, //www.curenaturalicancro.com/, deitar-se, hodgkin, //www.cancerfungus.com/, alcuni, //www.cancerfungus.com/br-blog-simoncini-cancer-fungos…, muitíssimos, 4-5, candidíases, salgar, metódica, dell'intestino, //www.medicinacomplementar.com.br/temanov08.asp, diffuso, empiricamente, dr., orientadas, uterina, metodicamente, suspendendo, 150-200, desintegra, /100, constatação, poderosíssima, semanas.4-5, adaptabilidade, 10/12/08, polmonari, cancerosas, reversões, bórax, cerebrali, gotejador, intertítulo, ”, comunicado-circular, tumori, dedicando, brônquios, //www.cancerfungus.com/simoncini-cancro-fungo.php, hepatocarcinoma, 3-4, obtinha, máfia-de-branco, //planogeral-marcosrocha.blogspot.com/…/descoberta-ovo…, piccoli, retal, recém-nascidos, candida, palpebra, midollare, •, metastasi.polmonari, '', seletiva, homeopático, //www.curenaturalicancro.org/…/adenocarcinoma_prostata…, esôfago, dosagens, alcalinizando, http, intracelular, vescica, 360°, entopem, subministrar, palpáveis, constatou, “, cobaltoterapia, trattati, diretaço, ½, cérvico-uterino, queimação, penetrarem, beneficiados, relatando, linfonodos, polmoni, coliciste, escorra, charlatões, macrobióticos, manifestam</t>
-  </si>
-  <si>
-    <t>japao, pergosa, adiquire, 40℅, transmissao, medicos</t>
-  </si>
-  <si>
-    <t>contribua, enviá-lo, e-mail, executá-lo, 19h25, escarro, espreitam, circulante, ​​e, ↗, ..., economizaremos, tossindo, arrastrar, cpr</t>
-  </si>
-  <si>
-    <t>esquente, lembre-se</t>
-  </si>
-  <si>
-    <t>parents, triplice, auto-imune, vaccination, outside, –, supreme, saudáveis​​, previnem, imunocomprometidas, empurrá-las, guide, age-, glutamato, vaers, studies, patrocinados, hpv, tetyana, sids, bulas, nauseam, placebos, prevalente, immunity, clinical, diseases, dizer-lhe, information, related, gms, matá-la, guillain-barré, ultrajantes, imunológica, .com, monossódico, concedem, defending, pró-vacina, vacinada, vactruth.com, responsabilizadas, esboçam, imuno-debilitados, lesadas, vaxtruth, reasons, isentando, unvaccinated, reactions, —, origins, transgênicos, concertado, ​​e, rentáveis, comprovadamente, adverse, ingredients, vaccinated, madness, sanevax, processadas, firms, empurradores-de-vacina, anvisa, incuráveis, harm, updated, injury, mandates, childhood, smallpox, impact, obukhanych, gardasil, ”, calá-los, u.s., infectious, vacinadas, //www.noticiasnaturais.com/…/10-razoes-pelas-quais-v…/…, vaccinate, figures, adjuvantes, liability, anulando-os, sgb, recommended, ogms, vaccines, guillain-barre, vactruth, pharma, reorientar, http, contraia, danificam, comprehensive, permitindo-lhe, higher, “, says, choose, ’, post-gardasil, afligidos, vaccine, illusion, ​​em, drug, healthier</t>
-  </si>
-  <si>
-    <t>estreitarem, progrida, esvaziamos, pode-se, aquecê-la, resfriada</t>
-  </si>
-  <si>
-    <t>almeido, cardiologia/secretaria, reparem…, usp, repassado, lembre-se, dr., soc.bras.de, conseqüente, ambev, ingerirem, fleury, e-mail, repassando, indenizar, parou…, fenofinol, “, …, internação, mídia…, ”, skol, voliteral</t>
-  </si>
-  <si>
-    <t>reddy, grapefruit, extrato, nutricionais, ..., '', batata-doce, dr., encaminhá-lo, 2-3, incentivei, guruprasad, insônia, morrem.., osh, 5-7, cancerosa, polifenol, handphone, cancerosas, xícaras, comprovaram, digeri-los, curativas, cítrico</t>
-  </si>
-  <si>
-    <t>'', repatriados, recusei-me, aconselhavam, ..., 'medicar-se, chama-se, wuhan, ``, acrescentando, coronavírus</t>
-  </si>
-  <si>
-    <t>elevem, '', wurhan, globalistas, soros, -o, alertamos, 2/3, começõu, rockfellers, jinping, gloso, ``, globalista, aglomerações, totall, rothschilds</t>
-  </si>
-  <si>
-    <t>alforjón, broto, gergelim, milheto, sorgo, documente, lembre-se, laetril, amígdalina, dr., contrabandeado, sabugueiro, absorvível, colonizador, compartilhe-o, tonsilar, *5, transformaram-na, brotos, b17, “, …, grumos, macadâmia, ”, *sementes, w., manner, derivada, descobriu-se</t>
-  </si>
-  <si>
-    <t>almeido, cardiologia/secretaria, reparem…, ..., usp, lembre-se, substancias, dr., soc.bras.de, conseqüente, ingerirem, fleury, repassando, indenizar, parou…, fenofinol, “, …, citados, internação, mídia…, ”, coca-cola, voliteral, repassada, repassem</t>
-  </si>
-  <si>
-    <t>'', esterilidade, vômitos, xampu, 5-10, uterina, ..., ``, lpki, abdome</t>
-  </si>
-  <si>
-    <t>aspirará, 16º, dar-se, incrementando, deve-se, especificam, disperse, deixá-las, excessivas, mg/929, minutos., mg., leva-se, aceitável…, c., “, 2000-4000, cm2, ”, 400-800, repassem</t>
-  </si>
-  <si>
-    <t>'', est.á, distribuíram, chama-se, ``, subornam</t>
-  </si>
-  <si>
-    <t>fatiados, poupadas, infecção…, protejam-se, descartei, salmonella, –, minimiza, estabilizantes, delete, camboriú-sc, ‘, superdivertida, draft, cevabacillus, 03/01/16, 08/01/16, camboriú, e-mail, coccus, fatie, sacarovictus, nociva, excessivos, noturnas, ’, muniz, organismo.., dermato, .., divulguem, ativus, cítrico</t>
-  </si>
-  <si>
-    <t>radioativas</t>
-  </si>
-  <si>
-    <t>influenza, erva-doce, tamiflu, c., repasse, famíliares, nossso, aconselha-se, 12/horas, acerola, h1n1, infectologista, –</t>
+    <t>vactruth.com, dizer-lhe, matá-la, permitindo-lhe, ​​e, vactruth, —, vaccinated, sanevax, empurrá-las, “, vaccination, vaxtruth, tetyana, calá-los, mandates, anulando-os, vaccines, age-, imunocomprometidas, vaccinate, unvaccinated, ”, ​​em, post-gardasil, empurradores-de-vacina, pró-vacina, saudáveis​​, imuno-debilitados, .com, vaers, guillain-barré, obukhanych, u.s., auto-imune, guillain-barre, –, ’, healthier</t>
+  </si>
+  <si>
+    <t>/100, professores-doutores-catedráticos-phds, peritoneale, semanas.4-5, 20-30-40, tumori, 90°, --, 36a, alcuni, vescica, baseia-se, engoli-la, “, coliciste, midollare, experimente-a, câncer/2008, 150-200, colecisti, ``, mês.1, difusível, removê-la, ovo-de-colombo, acidificando, •, turmores, comunicado-circular, candidíases, intertítulo, vezes.1, novembro/2008, dr., diffuso, 70-100, epatocarcinoma, 3-4, polmoni, ”, 'delete, bronchiale, alcalinizando, 360°, 10/12/08, pecezinho, trattati, complementá-la, cérvico-uterino, posicionar-se, nahco3, administrá-lo, carcinosi, polmonari, 4-5, máfia-de-branco, cerebrali, metastasi.polmonari, usa-se, ½, dias.3, cervice, deitar-se, caixa-postal, recém-nascidos, .todos, dell'intestino, cobaltoterapia, ..., não-hodgkin, '', 1/2</t>
+  </si>
+  <si>
+    <t>leva-se, deve-se, 16º, deixá-las, mg., ”, mg/929, “, aspirará, 2000-4000, cm2, minutos., c., dar-se, aceitável…, 400-800</t>
+  </si>
+  <si>
+    <t>``, colocá-la, 'se, 9,5, zerocal, 30º, carta-posição, dr., 3078-0995, h.j, arckle, assolassem, '', 9975-4476</t>
+  </si>
+  <si>
+    <t>lembre-se</t>
+  </si>
+  <si>
+    <t>aquecê-la, pode-se</t>
+  </si>
+  <si>
+    <t>'mistura, reparte-se, ...</t>
+  </si>
+  <si>
+    <t>aconselha-se, erva-doce, –, c., 12/horas, h1n1</t>
+  </si>
+  <si>
+    <t>e-mail, parou…, ”, ambev, “, reparem…, voliteral, …, soc.bras.de, cardiologia/secretaria, almeido, dr., fenofinol, mídia…, lembre-se</t>
+  </si>
+  <si>
+    <t>parou…, ”, “, reparem…, voliteral, …, soc.bras.de, cardiologia/secretaria, ..., coca-cola, dr., fenofinol, mídia…, almeido, lembre-se</t>
+  </si>
+  <si>
+    <t>5-7, morrem.., digeri-los, encaminhá-lo, '', batata-doce, 2-3, ..., dr., handphone, polifenol, guruprasad</t>
+  </si>
+  <si>
+    <t>amígdalina, ”, *5, descobriu-se, w., compartilhe-o, *sementes, …, “, b17, dr., transformaram-na, alforjón, lembre-se</t>
+  </si>
+  <si>
+    <t>outros…, 16h, 11h</t>
+  </si>
+  <si>
+    <t>``, 5-10, lpki, ..., ''</t>
+  </si>
+  <si>
+    <t>``, '', chama-se, est.á</t>
+  </si>
+  <si>
+    <t>e-mail, organismo.., ativus, protejam-se, .., sacarovictus, 03/01/16, cevabacillus, camboriú-sc, 08/01/16, infecção…, ‘, –, ’</t>
+  </si>
+  <si>
+    <t>30-50cc, 50-80cc, c.</t>
+  </si>
+  <si>
+    <t>pergosa, adiquire, 40℅</t>
+  </si>
+  <si>
+    <t>``, wurhan, 2/3, gloso, '', -o</t>
+  </si>
+  <si>
+    <t>enviá-lo, e-mail, ​​e, ↗, 19h25, ..., executá-lo</t>
+  </si>
+  <si>
+    <t>compartilhá-lo, tirei-a, ...</t>
+  </si>
+  <si>
+    <t>3-4, ademola, ..., afaste-se, lembre-se</t>
+  </si>
+  <si>
+    <t>'medicar-se, ``, recusei-me, ..., '', chama-se</t>
+  </si>
+  <si>
+    <t>huiren, ”, .., “, …</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>0.04119850187265917</v>
+        <v>0.02572559366754617</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -549,7 +546,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>0.01385041551246537</v>
+        <v>0.01526393894424422</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -560,7 +557,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>0.0273224043715847</v>
+        <v>0.04199475065616798</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -571,7 +568,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>0.01923076923076923</v>
+        <v>0.01506996770721206</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -582,7 +579,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>0.02222222222222222</v>
+        <v>0.009345794392523364</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -593,7 +590,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="1">
-        <v>0.04951560818083961</v>
+        <v>0.005747126436781609</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -604,7 +601,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="1">
-        <v>0.03418803418803419</v>
+        <v>0.004155124653739612</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -615,7 +612,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>0.03999158071984845</v>
+        <v>0.03508771929824561</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -626,7 +623,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="1">
-        <v>0.07317073170731707</v>
+        <v>0.05639097744360902</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -637,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="1">
-        <v>0.03303964757709251</v>
+        <v>0.04658385093167702</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -648,7 +645,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="1">
-        <v>0.01869158878504673</v>
+        <v>0.01854714064914992</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -659,7 +656,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="1">
-        <v>0.07439104674127715</v>
+        <v>0.01936376210235131</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -670,7 +667,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>0.01724137931034483</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -681,7 +678,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="1">
-        <v>0.09022556390977443</v>
+        <v>0.01644736842105263</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -692,7 +689,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="1">
-        <v>0.03863987635239567</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -703,7 +700,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="1">
-        <v>0.04313725490196078</v>
+        <v>0.02868852459016394</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -714,7 +711,7 @@
         <v>44</v>
       </c>
       <c r="C18" s="1">
-        <v>0.07834101382488479</v>
+        <v>0.01282051282051282</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -725,18 +722,15 @@
         <v>45</v>
       </c>
       <c r="C19" s="1">
-        <v>0.04149377593360996</v>
+        <v>0.03658536585365853</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
       <c r="C20" s="1">
-        <v>0.08074534161490683</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -744,10 +738,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1">
-        <v>0.03289473684210526</v>
+        <v>0.02764976958525346</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -755,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1">
-        <v>0.05511811023622047</v>
+        <v>0.01541850220264317</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -766,10 +760,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1">
-        <v>0.0576923076923077</v>
+        <v>0.008241758241758242</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -777,10 +771,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1">
-        <v>0.06762295081967214</v>
+        <v>0.0273224043715847</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -788,10 +782,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1">
-        <v>0.005208333333333333</v>
+        <v>0.02352941176470588</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -799,10 +793,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1">
-        <v>0.07602339181286549</v>
+        <v>0.01872659176029963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dictionary. Removed frequence less 100
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -100,76 +100,76 @@
     <t>Água quente com abacaxi.txt</t>
   </si>
   <si>
-    <t>vactruth.com, dizer-lhe, matá-la, permitindo-lhe, ​​e, vactruth, —, vaccinated, sanevax, empurrá-las, “, vaccination, vaxtruth, tetyana, calá-los, mandates, anulando-os, vaccines, age-, imunocomprometidas, vaccinate, unvaccinated, ”, ​​em, post-gardasil, empurradores-de-vacina, pró-vacina, saudáveis​​, imuno-debilitados, .com, vaers, guillain-barré, obukhanych, u.s., auto-imune, guillain-barre, –, ’, healthier</t>
-  </si>
-  <si>
-    <t>/100, professores-doutores-catedráticos-phds, peritoneale, semanas.4-5, 20-30-40, tumori, 90°, --, 36a, alcuni, vescica, baseia-se, engoli-la, “, coliciste, midollare, experimente-a, câncer/2008, 150-200, colecisti, ``, mês.1, difusível, removê-la, ovo-de-colombo, acidificando, •, turmores, comunicado-circular, candidíases, intertítulo, vezes.1, novembro/2008, dr., diffuso, 70-100, epatocarcinoma, 3-4, polmoni, ”, 'delete, bronchiale, alcalinizando, 360°, 10/12/08, pecezinho, trattati, complementá-la, cérvico-uterino, posicionar-se, nahco3, administrá-lo, carcinosi, polmonari, 4-5, máfia-de-branco, cerebrali, metastasi.polmonari, usa-se, ½, dias.3, cervice, deitar-se, caixa-postal, recém-nascidos, .todos, dell'intestino, cobaltoterapia, ..., não-hodgkin, '', 1/2</t>
-  </si>
-  <si>
-    <t>leva-se, deve-se, 16º, deixá-las, mg., ”, mg/929, “, aspirará, 2000-4000, cm2, minutos., c., dar-se, aceitável…, 400-800</t>
-  </si>
-  <si>
-    <t>``, colocá-la, 'se, 9,5, zerocal, 30º, carta-posição, dr., 3078-0995, h.j, arckle, assolassem, '', 9975-4476</t>
-  </si>
-  <si>
-    <t>lembre-se</t>
-  </si>
-  <si>
-    <t>aquecê-la, pode-se</t>
-  </si>
-  <si>
-    <t>'mistura, reparte-se, ...</t>
-  </si>
-  <si>
-    <t>aconselha-se, erva-doce, –, c., 12/horas, h1n1</t>
-  </si>
-  <si>
-    <t>e-mail, parou…, ”, ambev, “, reparem…, voliteral, …, soc.bras.de, cardiologia/secretaria, almeido, dr., fenofinol, mídia…, lembre-se</t>
-  </si>
-  <si>
-    <t>parou…, ”, “, reparem…, voliteral, …, soc.bras.de, cardiologia/secretaria, ..., coca-cola, dr., fenofinol, mídia…, almeido, lembre-se</t>
-  </si>
-  <si>
-    <t>5-7, morrem.., digeri-los, encaminhá-lo, '', batata-doce, 2-3, ..., dr., handphone, polifenol, guruprasad</t>
-  </si>
-  <si>
-    <t>amígdalina, ”, *5, descobriu-se, w., compartilhe-o, *sementes, …, “, b17, dr., transformaram-na, alforjón, lembre-se</t>
-  </si>
-  <si>
-    <t>outros…, 16h, 11h</t>
-  </si>
-  <si>
-    <t>``, 5-10, lpki, ..., ''</t>
-  </si>
-  <si>
-    <t>``, '', chama-se, est.á</t>
-  </si>
-  <si>
-    <t>e-mail, organismo.., ativus, protejam-se, .., sacarovictus, 03/01/16, cevabacillus, camboriú-sc, 08/01/16, infecção…, ‘, –, ’</t>
-  </si>
-  <si>
-    <t>30-50cc, 50-80cc, c.</t>
-  </si>
-  <si>
-    <t>pergosa, adiquire, 40℅</t>
-  </si>
-  <si>
-    <t>``, wurhan, 2/3, gloso, '', -o</t>
-  </si>
-  <si>
-    <t>enviá-lo, e-mail, ​​e, ↗, 19h25, ..., executá-lo</t>
-  </si>
-  <si>
-    <t>compartilhá-lo, tirei-a, ...</t>
-  </si>
-  <si>
-    <t>3-4, ademola, ..., afaste-se, lembre-se</t>
-  </si>
-  <si>
-    <t>'medicar-se, ``, recusei-me, ..., '', chama-se</t>
-  </si>
-  <si>
-    <t>huiren, ”, .., “, …</t>
+    <t>eficazmente, unvaccinated, incuráveis, responsabilizadas, tetyana, barré, gardasil, danificam, isentando, obukhanych, triplice, bulas, esboçam, patrocinados, –, prevalente, calá, lesadas, conservantes, razoes, comprovadamente, monossódico, vaxtruth, vaers, sgb, ​​e, nauseam, —, sanevax, guillain, empurradores, imuno, vactruth, afligidos, vacinadas, ​​em, vactruthcom, debilitados, matá, anvisa, adjuvantes, glutamato, concedem, ’, concertado, empurrá, saudáveis​​, contraia, imunocomprometidas, “, v…/…, gms, placebos, sids, previnem, imunológica, reorientar</t>
+  </si>
+  <si>
+    <t>linfomas, acidificando, entopem, dosagens, aftas, albicans, piccoli, catedráticos, mês1, metastasipolmonari, peritonial, novembro/2008, aproveitável, administrá, jfj, complementá, candidíase, peritoneale, colecisti, conjuntiva, carcinosi, metástases, 360°, coliciste, cancerologia, nahco3, epatocarcinoma, dellintestino, adaptabilidade, trattati, prostata, midollare, pecezinho, mangueirinha, 90°, gotejador, hepatocarcinoma, axilares, revolucionando, aprofundando, palpebra, cancerosas, penetrarem, embasamento, tumore, cérvico, muitíssimos, polmonari, bórax, cerebrali, semanas4, deleto, removê, charlatanismo, diretaço, câncer/2008, vescica, endossando, hodgkin, didática, ½, uterino, persistirem, salgar, alcuni, difusível, ingerível, casi, empiricamente, metodologias, especificas, subsequentemente, metodicamente, coróide, urinaria, marcosrochablogspotcom//descoberta, diffuso, adenocarcinoma, vezes1, oriundos, inalações, reversões, teclar, 10/12/08, arteriografia, percebíamos, candidíases, apregoam, simoncini, bronchiale, 5todos, brônquios, equimoses, integradores, alcalinizando, ministrando, homeopático, escorra, intracelular, •, 1/2, turmores, praticadas, cobaltoterapia, menstruações, linfonodos, tanti, subministrar, intertítulo, intersticial, polmoni, paradigmas, picaretagem, palpáveis, 36a, orientadas, poderosíssima, /100, cervice, obtinha, constatou, homeopatia, lincados, dias3, tumori, “, fungophp, oncologistas, macrobióticos, vari</t>
+  </si>
+  <si>
+    <t>mg/929, “, incrementando, aspirará, cm2, 16º, especificam, aceitável…, repassem</t>
+  </si>
+  <si>
+    <t>fibromialgia, aspartame, agravando, comercializem, adiposas, assintomáticas, internadas, colocá, riccio, 30º, engaje, mancy, fórmico, fetais, nutrasweet, dietética, assolassem, arckle, malformações, dietético, suplanta, sistêmico, articulares, entitulado, zerocal</t>
+  </si>
+  <si>
+    <t>partilhem</t>
+  </si>
+  <si>
+    <t>aquecê, progrida, estreitarem, lugarquando, esvaziamos</t>
+  </si>
+  <si>
+    <t>menstruais, solidifica, obstipação, vómitos, reparte</t>
+  </si>
+  <si>
+    <t>–, tamiflu, nossso, acerola, h1n1, famíliares, 12/horas, infectologista</t>
+  </si>
+  <si>
+    <t>cardiologia/secretaria, socbrasde, fenofinol, teixeira, ambev, indenizar, “, freitas, ingerirem, usp, almeido, repassado, conseqüente, voliteral</t>
+  </si>
+  <si>
+    <t>proprios, socbrasde, cardiologia/secretaria, voliteral, fenofinol, teixeira, indenizar, repassada, “, freitas, ingerirem, substancias, usp, almeido, conseqüente, repassem</t>
+  </si>
+  <si>
+    <t>osh, encaminhá, cancerosa, cancerosas, curativas, incentivei, comprovaram, digeri, handphone, polifenol, guruprasad</t>
+  </si>
+  <si>
+    <t>alforjón, b17, laetril, sabugueiro, sorgo, documente, macadâmia, “, grumos, rebentos, amígdalina, absorvível, 5sementes, tonsilar, milheto, colonizador</t>
+  </si>
+  <si>
+    <t>11h, indicativos, 16h</t>
+  </si>
+  <si>
+    <t>lpki</t>
+  </si>
+  <si>
+    <t>subornam, distribuíram, partilhe</t>
+  </si>
+  <si>
+    <t>superdivertida, cevabacillus, muniz, fatie, ativus, –, conservantes, internamento, divulguem, camboriú, coccus, estabilizantes, sacarovictus, ‘, 03/01/16, 08/01/16, ’, fatiados, minimiza, dermato</t>
+  </si>
+  <si>
+    <t>80cc, coronavírus, 50cc, invadirá</t>
+  </si>
+  <si>
+    <t>medicos, afectados, informaçao, adiquire, pergosa, japao, transmissao</t>
+  </si>
+  <si>
+    <t>globalista, totall, começõu, wurhan, elevem, jinping, aglomerações, rockfellers, globalistas, soros, gloso, rothschilds, 2/3</t>
+  </si>
+  <si>
+    <t>economizaremos, arrastrar, circulante, executá, escarro, 19h25, enviá, ​​e</t>
+  </si>
+  <si>
+    <t>compartilhá, reencaminhado</t>
+  </si>
+  <si>
+    <t>partilhou, ademola</t>
+  </si>
+  <si>
+    <t>coronavírus, wuhan, aconselhavam, repatriados</t>
+  </si>
+  <si>
+    <t>alcalina, anticâncer, huiren, polifenóis, “, enfatizou, cistos</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>0.02572559366754617</v>
+        <v>0.03988803358992302</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -546,7 +546,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>0.01526393894424422</v>
+        <v>0.03083491461100569</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -557,7 +557,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>0.04199475065616798</v>
+        <v>0.02593659942363112</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -568,7 +568,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>0.01506996770721206</v>
+        <v>0.03019323671497584</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -579,7 +579,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>0.009345794392523364</v>
+        <v>0.0101010101010101</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -590,7 +590,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="1">
-        <v>0.005747126436781609</v>
+        <v>0.01633986928104575</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -601,7 +601,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="1">
-        <v>0.004155124653739612</v>
+        <v>0.008183306055646482</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -612,7 +612,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>0.03508771929824561</v>
+        <v>0.05128205128205128</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -623,7 +623,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="1">
-        <v>0.05639097744360902</v>
+        <v>0.05857740585774059</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="1">
-        <v>0.04658385093167702</v>
+        <v>0.05614035087719298</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -645,7 +645,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="1">
-        <v>0.01854714064914992</v>
+        <v>0.01906412478336222</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -656,7 +656,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="1">
-        <v>0.01936376210235131</v>
+        <v>0.02531645569620253</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -667,7 +667,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>0.01333333333333333</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -678,7 +678,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="1">
-        <v>0.01644736842105263</v>
+        <v>0.003759398496240601</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -689,7 +689,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="1">
-        <v>0.03846153846153846</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -700,7 +700,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="1">
-        <v>0.02868852459016394</v>
+        <v>0.04608294930875576</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -711,7 +711,7 @@
         <v>44</v>
       </c>
       <c r="C18" s="1">
-        <v>0.01282051282051282</v>
+        <v>0.0196078431372549</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -722,7 +722,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="1">
-        <v>0.03658536585365853</v>
+        <v>0.0958904109589041</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -741,7 +741,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="1">
-        <v>0.02764976958525346</v>
+        <v>0.0755813953488372</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -752,7 +752,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="1">
-        <v>0.01541850220264317</v>
+        <v>0.0199501246882793</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -763,7 +763,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="1">
-        <v>0.008241758241758242</v>
+        <v>0.006042296072507553</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -774,7 +774,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1">
-        <v>0.0273224043715847</v>
+        <v>0.01162790697674419</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -785,7 +785,7 @@
         <v>50</v>
       </c>
       <c r="C25" s="1">
-        <v>0.02352941176470588</v>
+        <v>0.01801801801801802</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -796,7 +796,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="1">
-        <v>0.01872659176029963</v>
+        <v>0.03043478260869565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spell checker finished (?)
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Texto</t>
   </si>
@@ -100,76 +100,73 @@
     <t>Água quente com abacaxi.txt</t>
   </si>
   <si>
-    <t>eficazmente, unvaccinated, incuráveis, responsabilizadas, tetyana, barré, gardasil, danificam, isentando, obukhanych, triplice, bulas, esboçam, patrocinados, –, prevalente, calá, lesadas, conservantes, razoes, comprovadamente, monossódico, vaxtruth, vaers, sgb, ​​e, nauseam, —, sanevax, guillain, empurradores, imuno, vactruth, afligidos, vacinadas, ​​em, vactruthcom, debilitados, matá, anvisa, adjuvantes, glutamato, concedem, ’, concertado, empurrá, saudáveis​​, contraia, imunocomprometidas, “, v…/…, gms, placebos, sids, previnem, imunológica, reorientar</t>
-  </si>
-  <si>
-    <t>linfomas, acidificando, entopem, dosagens, aftas, albicans, piccoli, catedráticos, mês1, metastasipolmonari, peritonial, novembro/2008, aproveitável, administrá, jfj, complementá, candidíase, peritoneale, colecisti, conjuntiva, carcinosi, metástases, 360°, coliciste, cancerologia, nahco3, epatocarcinoma, dellintestino, adaptabilidade, trattati, prostata, midollare, pecezinho, mangueirinha, 90°, gotejador, hepatocarcinoma, axilares, revolucionando, aprofundando, palpebra, cancerosas, penetrarem, embasamento, tumore, cérvico, muitíssimos, polmonari, bórax, cerebrali, semanas4, deleto, removê, charlatanismo, diretaço, câncer/2008, vescica, endossando, hodgkin, didática, ½, uterino, persistirem, salgar, alcuni, difusível, ingerível, casi, empiricamente, metodologias, especificas, subsequentemente, metodicamente, coróide, urinaria, marcosrochablogspotcom//descoberta, diffuso, adenocarcinoma, vezes1, oriundos, inalações, reversões, teclar, 10/12/08, arteriografia, percebíamos, candidíases, apregoam, simoncini, bronchiale, 5todos, brônquios, equimoses, integradores, alcalinizando, ministrando, homeopático, escorra, intracelular, •, 1/2, turmores, praticadas, cobaltoterapia, menstruações, linfonodos, tanti, subministrar, intertítulo, intersticial, polmoni, paradigmas, picaretagem, palpáveis, 36a, orientadas, poderosíssima, /100, cervice, obtinha, constatou, homeopatia, lincados, dias3, tumori, “, fungophp, oncologistas, macrobióticos, vari</t>
-  </si>
-  <si>
-    <t>mg/929, “, incrementando, aspirará, cm2, 16º, especificam, aceitável…, repassem</t>
-  </si>
-  <si>
-    <t>fibromialgia, aspartame, agravando, comercializem, adiposas, assintomáticas, internadas, colocá, riccio, 30º, engaje, mancy, fórmico, fetais, nutrasweet, dietética, assolassem, arckle, malformações, dietético, suplanta, sistêmico, articulares, entitulado, zerocal</t>
-  </si>
-  <si>
-    <t>partilhem</t>
-  </si>
-  <si>
-    <t>aquecê, progrida, estreitarem, lugarquando, esvaziamos</t>
-  </si>
-  <si>
-    <t>menstruais, solidifica, obstipação, vómitos, reparte</t>
-  </si>
-  <si>
-    <t>–, tamiflu, nossso, acerola, h1n1, famíliares, 12/horas, infectologista</t>
-  </si>
-  <si>
-    <t>cardiologia/secretaria, socbrasde, fenofinol, teixeira, ambev, indenizar, “, freitas, ingerirem, usp, almeido, repassado, conseqüente, voliteral</t>
-  </si>
-  <si>
-    <t>proprios, socbrasde, cardiologia/secretaria, voliteral, fenofinol, teixeira, indenizar, repassada, “, freitas, ingerirem, substancias, usp, almeido, conseqüente, repassem</t>
-  </si>
-  <si>
-    <t>osh, encaminhá, cancerosa, cancerosas, curativas, incentivei, comprovaram, digeri, handphone, polifenol, guruprasad</t>
-  </si>
-  <si>
-    <t>alforjón, b17, laetril, sabugueiro, sorgo, documente, macadâmia, “, grumos, rebentos, amígdalina, absorvível, 5sementes, tonsilar, milheto, colonizador</t>
-  </si>
-  <si>
-    <t>11h, indicativos, 16h</t>
+    <t>previnem, reactions, recommended, saudáveis​​, anvisa, triplice, obukhanych, vaxtruth, vaccinated, transgênicos, unvaccinated, mandates, empurradores, ​​e, nauseam, vaers, reorientar, studies, ogms, sites, –, tetyana, healthier, defending, ’, vactruthcom, gardasil, diseases, sgb, pharma, parents, says, reasons, report, gms, comprovadamente, ingredients, updated, “, eficazmente, sanevax, vaccines, higher, —, imunocomprometidas, ​​em, origins, rentáveis, injury, vactruth, related, firms</t>
+  </si>
+  <si>
+    <t>diretaço, bronchiale, adaptabilidade, phds, sites, coróide, subsequentemente, colecisti, linfomas, jfj, candidíases, epatocarcinoma, tumore, ingerível, deleto, adequadamente, turmores, trattati, pediátrica, nahco3, alla, è, macrobióticos, carcinosi, peritoneale, estomago, alcalinizando, vescica, charcot, polmonari, tullio, “, metodicamente, piccoli, prostata, poderosíssima, pazes, metastasipolmonari, pessoalmente, 360°, reversões, restringe, cânceres, polmoni, dias3, pecezinho, •, diffuso, simoncini, gotejador, links, 90°, intertítulo, cerebrali, absurdamente, abrasões, casi, lincados, subministrar, tanti, cérvico, entopem, 5todos, semanas4, espetaculares, alcuni, coliciste, dellintestino, vezes1, mês1, oncologista, ½, inalador, legendado, tumori, radiografias, palpebra, midollare, oncologistas, 36a</t>
+  </si>
+  <si>
+    <t>refrescante, 16º, cm2, “, simplemente</t>
+  </si>
+  <si>
+    <t>adoçante, blaylock, 30º, arckle, entitulado, atenciosamente, câimbras, mancy, zerocal, dopamina, riccio, hj, raffaele, lobbies</t>
+  </si>
+  <si>
+    <t>possivel</t>
+  </si>
+  <si>
+    <t>cairam, lugarquando</t>
+  </si>
+  <si>
+    <t>reage, vómitos</t>
+  </si>
+  <si>
+    <t>infectologista, –, nossso, tamiflu, famíliares, h1n1</t>
+  </si>
+  <si>
+    <t>fenofinol, socbrasde, ambev, “, voliteral, skol, fleury, almeido</t>
+  </si>
+  <si>
+    <t>fenofinol, fanta, socbrasde, “, voliteral, proprios, fleury, almeido</t>
+  </si>
+  <si>
+    <t>osh, polifenol, guruprasad, handphone, reddy</t>
+  </si>
+  <si>
+    <t>laetril, mirtilos, “, alforjón, b17, amígdalina, 5sementes</t>
+  </si>
+  <si>
+    <t>11h, 16h</t>
   </si>
   <si>
     <t>lpki</t>
   </si>
   <si>
-    <t>subornam, distribuíram, partilhe</t>
-  </si>
-  <si>
-    <t>superdivertida, cevabacillus, muniz, fatie, ativus, –, conservantes, internamento, divulguem, camboriú, coccus, estabilizantes, sacarovictus, ‘, 03/01/16, 08/01/16, ’, fatiados, minimiza, dermato</t>
-  </si>
-  <si>
-    <t>80cc, coronavírus, 50cc, invadirá</t>
-  </si>
-  <si>
-    <t>medicos, afectados, informaçao, adiquire, pergosa, japao, transmissao</t>
-  </si>
-  <si>
-    <t>globalista, totall, começõu, wurhan, elevem, jinping, aglomerações, rockfellers, globalistas, soros, gloso, rothschilds, 2/3</t>
-  </si>
-  <si>
-    <t>economizaremos, arrastrar, circulante, executá, escarro, 19h25, enviá, ​​e</t>
-  </si>
-  <si>
-    <t>compartilhá, reencaminhado</t>
-  </si>
-  <si>
-    <t>partilhou, ademola</t>
-  </si>
-  <si>
-    <t>coronavírus, wuhan, aconselhavam, repatriados</t>
-  </si>
-  <si>
-    <t>alcalina, anticâncer, huiren, polifenóis, “, enfatizou, cistos</t>
+    <t>sacarovictus, prontamente, superdivertida, –, ‘, aconchegante, ’, cevabacillus, ativus, humildemente, libre, contactei</t>
+  </si>
+  <si>
+    <t>50cc, desconfortáveis, 80cc</t>
+  </si>
+  <si>
+    <t>informaçao, podera, transmissao, afectados, japao, pergosa, adiquire, nao, estao, medicos</t>
+  </si>
+  <si>
+    <t>começõu, globalista, wurhan, rothschilds, rockfellers, lives, globalistas, alcool, jinping, totall</t>
+  </si>
+  <si>
+    <t>19h25, ​​e</t>
+  </si>
+  <si>
+    <t>reencaminhado</t>
+  </si>
+  <si>
+    <t>ademola, familiares</t>
+  </si>
+  <si>
+    <t>inalador</t>
+  </si>
+  <si>
+    <t>huiren, cistos, polifenóis, “, familiares, anticâncer</t>
   </si>
 </sst>
 </file>
@@ -535,7 +532,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>0.03988803358992302</v>
+        <v>0.03649122807017544</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -546,7 +543,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>0.03083491461100569</v>
+        <v>0.01900688999762414</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -557,7 +554,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>0.02593659942363112</v>
+        <v>0.01436781609195402</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -568,7 +565,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>0.03019323671497584</v>
+        <v>0.01690821256038647</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -590,7 +587,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="1">
-        <v>0.01633986928104575</v>
+        <v>0.006557377049180328</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -601,7 +598,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="1">
-        <v>0.008183306055646482</v>
+        <v>0.003273322422258593</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -612,7 +609,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>0.05128205128205128</v>
+        <v>0.03821656050955414</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -623,7 +620,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="1">
-        <v>0.05857740585774059</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -634,7 +631,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="1">
-        <v>0.05614035087719298</v>
+        <v>0.02797202797202797</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -645,7 +642,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="1">
-        <v>0.01906412478336222</v>
+        <v>0.008665511265164644</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -656,7 +653,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="1">
-        <v>0.02531645569620253</v>
+        <v>0.01107594936708861</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -667,7 +664,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>0.015</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -685,11 +682,8 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
       <c r="C16" s="1">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -697,10 +691,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1">
-        <v>0.04608294930875576</v>
+        <v>0.0273972602739726</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -708,10 +702,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1">
-        <v>0.0196078431372549</v>
+        <v>0.01477832512315271</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -719,10 +713,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1">
-        <v>0.0958904109589041</v>
+        <v>0.136986301369863</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -738,10 +732,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1">
-        <v>0.0755813953488372</v>
+        <v>0.05747126436781609</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -749,10 +743,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1">
-        <v>0.0199501246882793</v>
+        <v>0.004987531172069825</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -760,10 +754,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1">
-        <v>0.006042296072507553</v>
+        <v>0.003021148036253776</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -771,7 +765,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1">
         <v>0.01162790697674419</v>
@@ -782,10 +776,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1">
-        <v>0.01801801801801802</v>
+        <v>0.004504504504504504</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -793,10 +787,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1">
-        <v>0.03043478260869565</v>
+        <v>0.02608695652173913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix results on xlsx
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -28,7 +28,7 @@
     <t>Quantidade de palavras</t>
   </si>
   <si>
-    <t>Quantidade de paragrafos</t>
+    <t>Quantidade de parágrafos</t>
   </si>
   <si>
     <t>Solicita compartilhamento?</t>
@@ -184,19 +184,19 @@
     <t>Óleo no umbigo cura doenças.txt</t>
   </si>
   <si>
-    <t>vaers, unvaccinated, vactruthcom, recommended, anvisa, healthier, higher, nauseam, rentáveis, conservantes, afligidos, defending, sanevax, “, says, ​​em, gms, gardasil, imunocomprometidas, lesadas, obukhanych, tetyana, sgb, adjuvantes, updated, studies, comprovadamente, related, ogms, saudáveis​​, —, sites, injury, empurradores, transgênicos, patrocinados, nutrientes, vaccinated, eficazmente, responsabilizadas, origins, geneticamente, reorientar, vaxtruth, diseases, mandates, contêm, ingredients, placebos, reactions, parents, vaccines, firms, triplice, reasons, vactruth, ​​e, pharma</t>
-  </si>
-  <si>
-    <t>bronchiale, reversões, pecezinho, substancialmente, “, oncologista, diretaço, linfonodos, simoncini, cancerígenas, poderosíssima, piccoli, radiografias, conseqüência, 5todos, empiricamente, ingerível, entopem, alla, alcalinizando, coróide, gotejador, alcuni, pediátrica, nahco3, convincentes, 90°, midollare, metodologias, deleto, carcinosi, estomago, oncologistas, sites, cerebrali, metodicamente, vezes1, 36a, epatocarcinoma, restringe, peritoneale, candidíases, trattati, •, è, cânceres, legendado, cérvico, dias3, cirurgias, linfomas, turmores, lincados, dellintestino, lavagens, prostata, palpebra, colecisti, coliciste, tumore, links, inalador, casi, tumori, tanti, subministrar, vescica, inalações, polmonari, metastasipolmonari, 360°, diffuso, absurdamente, abrasões, macrobióticos, jfj, intertítulo, ½, equimoses, semanas4, metástases, sinceramente, adaptabilidade, enlouquecida, polmoni, mês1, phds, charcot</t>
-  </si>
-  <si>
-    <t>132ph, 87ph, 99ph, 85ph, 156ph, 227ph, 92ph, abençoê, 127ph</t>
-  </si>
-  <si>
-    <t>cm2, “, refrescante, simplemente, 16º</t>
-  </si>
-  <si>
-    <t>acidose, zerocal, raffaele, arckle, assintomáticas, dopamina, blaylock, mancy, 30º, contaminados, câimbras, entitulado, adoçante, riccio, lobbies, hj</t>
+    <t>nauseam, tetyana, vactruthcom, conservantes, sgb, responsabilizadas, updated, obukhanych, ogms, sites, ingredients, origins, triplice, vaccines, contêm, recommended, reorientar, adjuvantes, gardasil, injury, related, rentáveis, comprovadamente, empurradores, reasons, parents, vactruth, firms, unvaccinated, saudáveis​​, ​​em, eficazmente, mandates, healthier, vaers, geneticamente, studies, reactions, anvisa, vaxtruth, nutrientes, pharma, gms, vaccinated, defending, sanevax, diseases, afligidos, —, placebos, says, ​​e, lesadas, higher, imunocomprometidas, “, transgênicos, patrocinados</t>
+  </si>
+  <si>
+    <t>sites, midollare, coliciste, 5todos, estomago, palpebra, metodologias, equimoses, 36a, alcuni, tanti, simoncini, cancerígenas, sinceramente, carcinosi, inalações, gotejador, adaptabilidade, casi, peritoneale, tumori, oncologista, entopem, •, turmores, conseqüência, legendado, 90°, lincados, tumore, trattati, linfonodos, cânceres, pediátrica, piccoli, è, jfj, radiografias, diffuso, absurdamente, semanas4, ingerível, charcot, metastasipolmonari, cerebrali, bronchiale, oncologistas, phds, substancialmente, dellintestino, lavagens, reversões, vescica, prostata, abrasões, pecezinho, nahco3, 360°, deleto, coróide, cérvico, inalador, polmonari, macrobióticos, empiricamente, mês1, “, dias3, polmoni, links, convincentes, poderosíssima, candidíases, alla, metodicamente, metástases, intertítulo, subministrar, restringe, cirurgias, linfomas, colecisti, diretaço, epatocarcinoma, alcalinizando, vezes1, enlouquecida, ½</t>
+  </si>
+  <si>
+    <t>132ph, 87ph, 85ph, 127ph, 92ph, 99ph, abençoê, 227ph, 156ph</t>
+  </si>
+  <si>
+    <t>simplemente, 16º, refrescante, “, cm2</t>
+  </si>
+  <si>
+    <t>raffaele, 30º, contaminados, adoçante, hj, entitulado, riccio, assintomáticas, lobbies, blaylock, dopamina, mancy, arckle, acidose, zerocal, câimbras</t>
   </si>
   <si>
     <t>possivel</t>
@@ -211,73 +211,73 @@
     <t>infectologista</t>
   </si>
   <si>
-    <t>reage, vómitos</t>
+    <t>vómitos, reage</t>
   </si>
   <si>
     <t>percursso, hu</t>
   </si>
   <si>
-    <t>covid, wenliang, theophylline, “, methylxanthine, metilxantinas, theobromine</t>
-  </si>
-  <si>
-    <t>nossso, famíliares, h1n1, infectologista</t>
-  </si>
-  <si>
-    <t>covid, alcalinizam, comprovadamente, covid19</t>
+    <t>methylxanthine, theophylline, theobromine, covid, metilxantinas, wenliang, “</t>
+  </si>
+  <si>
+    <t>h1n1, nossso, infectologista, famíliares</t>
+  </si>
+  <si>
+    <t>alcalinizam, covid, comprovadamente, covid19</t>
   </si>
   <si>
     <t>covid, infectados</t>
   </si>
   <si>
-    <t>socbrasde, ambev, fleury, conseqüente, skol, tranqüila, almeido, “, voliteral, fenofinol</t>
-  </si>
-  <si>
-    <t>socbrasde, proprios, fleury, conseqüente, tranqüila, almeido, “, refrigerantes, fanta, voliteral, fenofinol</t>
+    <t>voliteral, tranqüila, almeido, skol, ambev, conseqüente, “, fenofinol, socbrasde, fleury</t>
+  </si>
+  <si>
+    <t>voliteral, tranqüila, almeido, fanta, refrigerantes, proprios, conseqüente, “, fenofinol, socbrasde, fleury</t>
   </si>
   <si>
     <t>desinfetante, mícrons, °</t>
   </si>
   <si>
-    <t>curativas, cancerígenas, guruprasad, trombose, handphone, osh, polifenol, reddy</t>
-  </si>
-  <si>
-    <t>obtêm, itens, b17, laetril, alforjón, “, 5sementes, amígdalina, mirtilos</t>
-  </si>
-  <si>
-    <t>sémen, infectada, 300cl, bph, acção, hormonais, 60cl, “, desconfortável, encanador, crónica, vestuario, wahala, , projectada, alguém…, cancerígenas, reembalar, afecta, boxers, extracto, canalizador, 15mg, dey, celibatos, jacto, canalizacao, directamente, hesistência, ugbogulu, horin, humedecimento, colega…, afectará, 50cl, atinge, cânceres, lawma, cancerígenos</t>
-  </si>
-  <si>
-    <t>16h, freqüente, 11h</t>
-  </si>
-  <si>
-    <t>crmsp33006, fenilpropalamina, ‘</t>
+    <t>polifenol, guruprasad, reddy, curativas, cancerígenas, handphone, trombose, osh</t>
+  </si>
+  <si>
+    <t>laetril, 5sementes, b17, obtêm, itens, “, mirtilos, alforjón, amígdalina</t>
+  </si>
+  <si>
+    <t>boxers, bph, canalizador, sémen, infectada, directamente, hormonais, humedecimento, lawma, hesistência, celibatos, afectará, 15mg, 50cl, dey, canalizacao, jacto, 300cl, cânceres, afecta, desconfortável, acção, wahala, reembalar, encanador, atinge, cancerígenas, 60cl, extracto, , crónica, projectada, horin, vestuario, colega…, “, cancerígenos, alguém…, ugbogulu</t>
+  </si>
+  <si>
+    <t>freqüente, 11h, 16h</t>
+  </si>
+  <si>
+    <t>‘, fenilpropalamina, crmsp33006</t>
   </si>
   <si>
     <t>lpki</t>
   </si>
   <si>
-    <t>horin, cancerígenas, tchen, monoalcólico</t>
-  </si>
-  <si>
-    <t>libre, fatiados, sacarovictus, humildemente, contactei, conservantes, superdivertida, aconchegante, ‘, cevabacillus, ativus, estabilizantes</t>
-  </si>
-  <si>
-    <t>80cc, 50cc, desconfortáveis</t>
-  </si>
-  <si>
-    <t>estao, japao, pergosa, adiquire, transmissao, nao, medicos, podera, informaçao, afectados</t>
-  </si>
-  <si>
-    <t>unitriedubr, cientifico, esculentus, extraida, “, unicampbr</t>
-  </si>
-  <si>
-    <t>globalista, rothschilds, totall, alcool, rockfellers, globalistas, jinping, começõu, infectados, lives, wurhan</t>
-  </si>
-  <si>
-    <t>desinfecte, cardiovasculares, puxadores, shenzhen, °, castello, cátaros, desinfetante, trombose, polmonite, drsse</t>
-  </si>
-  <si>
-    <t>mantêm, indevidamente, respirações, 19h25, gentilmente, ​​e</t>
+    <t>horin, tchen, monoalcólico, cancerígenas</t>
+  </si>
+  <si>
+    <t>libre, conservantes, sacarovictus, ‘, superdivertida, contactei, estabilizantes, humildemente, aconchegante, cevabacillus, fatiados, ativus</t>
+  </si>
+  <si>
+    <t>desconfortáveis, 50cc, 80cc</t>
+  </si>
+  <si>
+    <t>informaçao, transmissao, podera, pergosa, nao, medicos, estao, japao, afectados, adiquire</t>
+  </si>
+  <si>
+    <t>extraida, unicampbr, unitriedubr, esculentus, “, cientifico</t>
+  </si>
+  <si>
+    <t>wurhan, começõu, lives, rockfellers, totall, rothschilds, globalista, infectados, globalistas, jinping, alcool</t>
+  </si>
+  <si>
+    <t>desinfecte, polmonite, castello, puxadores, cátaros, drsse, °, trombose, shenzhen, desinfetante, cardiovasculares</t>
+  </si>
+  <si>
+    <t>indevidamente, mantêm, ​​e, respirações, gentilmente, 19h25</t>
   </si>
   <si>
     <t>reencaminhado, antioxidantes</t>
@@ -286,43 +286,43 @@
     <t>ademola</t>
   </si>
   <si>
-    <t>irreversível, bakkano, eletromagnetica</t>
+    <t>eletromagnetica, bakkano, irreversível</t>
   </si>
   <si>
     <t>repatriados, inalador</t>
   </si>
   <si>
-    <t>barbuto, oncologista, brasileirosuma, —, genoma</t>
-  </si>
-  <si>
-    <t>garganta…, varella</t>
-  </si>
-  <si>
-    <t>corrimãos, 2a, shenzen, 27°, letala, dágua</t>
-  </si>
-  <si>
-    <t>polifenóis, cistos, anticâncer, cancerígenas, huiren, “</t>
-  </si>
-  <si>
-    <t>opsdigo, 5g, naite, contaminados</t>
+    <t>oncologista, —, brasileirosuma, genoma, barbuto</t>
+  </si>
+  <si>
+    <t>varella, garganta…</t>
+  </si>
+  <si>
+    <t>shenzen, 27°, 2a, corrimãos, dágua, letala</t>
+  </si>
+  <si>
+    <t>polifenóis, cistos, cancerígenas, “, anticâncer, huiren</t>
+  </si>
+  <si>
+    <t>5g, contaminados, naite, opsdigo</t>
   </si>
   <si>
     <t>honjo, tasuku</t>
   </si>
   <si>
-    <t>guidelines, nissen, acc, americans, corticosteróides, _temos, cardiovasculares, dgac, framingham, coronariana, “</t>
-  </si>
-  <si>
-    <t>covid, eucalyptol, mentolatum, epoxi</t>
-  </si>
-  <si>
-    <t>chicungunha, sudoríparas, repasando, causador</t>
+    <t>americans, _temos, cardiovasculares, coronariana, guidelines, nissen, corticosteróides, “, acc, dgac, framingham</t>
+  </si>
+  <si>
+    <t>eucalyptol, mentolatum, epoxi, covid</t>
+  </si>
+  <si>
+    <t>repasando, sudoríparas, causador, chicungunha</t>
   </si>
   <si>
     <t>conscientemente</t>
   </si>
   <si>
-    <t>letargiaalívio, pechotique, naturista, ricino, nutrientes, hidratando, massagea, 4cm</t>
+    <t>nutrientes, hidratando, letargiaalívio, pechotique, massagea, naturista, ricino, 4cm</t>
   </si>
   <si>
     <t>sem compartilhamento</t>
@@ -331,7 +331,7 @@
     <t>compartilhamento</t>
   </si>
   <si>
-    <t>Acuracia: 64.1025641025641%</t>
+    <t>Acurácia: 64.1025641025641%</t>
   </si>
   <si>
     <t>não sensacionalista</t>
@@ -340,7 +340,7 @@
     <t>sensacionalista</t>
   </si>
   <si>
-    <t>Acuracia: 100.0%</t>
+    <t>Acurácia: 100.0%</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -685,10 +685,10 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="100.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="100.7109375" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" customWidth="1"/>
-    <col min="6" max="6" width="60.7109375" customWidth="1"/>
-    <col min="7" max="7" width="60.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1535,9 +1535,17 @@
         <v>0.02439024390243903</v>
       </c>
       <c r="F50" t="s">
+        <v>103</v>
+      </c>
+      <c r="G50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="F51" t="s">
         <v>105</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>